<commit_message>
Cambios al reproducir canciones
</commit_message>
<xml_diff>
--- a/tests_csv/deleted_songs.xlsx
+++ b/tests_csv/deleted_songs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlos/Documents/MCCIPN/2Sem/Seminario2/shazam/tests_csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04608C78-509D-5345-B92E-57D2CE312245}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FB252F-456C-5C46-942C-E5BCA261ADEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{107196CD-0CB0-2342-A8B5-60E40D0B8C76}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Nombre cancion</t>
   </si>
@@ -34,6 +34,15 @@
   </si>
   <si>
     <t>Archivo dañado</t>
+  </si>
+  <si>
+    <t>098619 es la misma canción y mismo fragmento</t>
+  </si>
+  <si>
+    <t>Dura 1 segundo</t>
+  </si>
+  <si>
+    <t>No tiene sonido alguno</t>
   </si>
 </sst>
 </file>
@@ -392,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{812A31AA-DDD7-924F-9520-189C65EE383E}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -478,6 +487,72 @@
         <v>2</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>133297</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>98617</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>98565</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>98567</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>98569</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>72059</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>